<commit_message>
Apache POI library dependency new version updated add
</commit_message>
<xml_diff>
--- a/Maven_Block_Armour/src/main/resources/Data/Block1.xlsx
+++ b/Maven_Block_Armour/src/main/resources/Data/Block1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\OneDrive\Desktop\Automation notes\Block_Armor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3407D018-905F-4CCC-9838-7239CE9DFD6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A769785-948C-4CE4-BA61-7DE3ADDFB6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{815AFF53-8EF9-4EA6-BFEF-E11D64647A81}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>UserName</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Pass@2023</t>
-  </si>
-  <si>
-    <t>ss</t>
   </si>
 </sst>
 </file>
@@ -797,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84626649-3FD1-4A78-B3B4-091287839029}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,7 +933,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>123458</v>
       </c>
@@ -944,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -952,8 +949,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -961,7 +958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
@@ -969,7 +966,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>14</v>
       </c>
@@ -977,7 +974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
@@ -985,7 +982,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -993,7 +990,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>12340</v>
       </c>
@@ -1009,7 +1006,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>16</v>
       </c>
@@ -1017,7 +1014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>17</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>13</v>
       </c>
@@ -1033,12 +1030,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
@@ -1046,15 +1043,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="F32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>